<commit_message>
Added raw data (Dates) and created a new plot for temporal pattern
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/TCSA_raw_data.xlsx
+++ b/analysis/data/raw_data/TCSA_raw_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gayoungp/CTtps/analysis/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gayoungp/Desktop/tcsakoreanpaleolithic/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18BD505-FD80-4F4C-8C6C-F09AE1C6E38B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C15FFA3-5D0D-094A-9D6C-79052842167B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22720" yWindow="820" windowWidth="25080" windowHeight="19400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6220" yWindow="7320" windowWidth="25080" windowHeight="19400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1572" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1572" uniqueCount="356">
   <si>
     <t>Region</t>
   </si>
@@ -1075,9 +1075,6 @@
     <t>Juksan</t>
   </si>
   <si>
-    <t>Site_name_detailed</t>
-  </si>
-  <si>
     <t>Suyanggae</t>
   </si>
   <si>
@@ -1085,6 +1082,12 @@
   </si>
   <si>
     <t>Sinbuk</t>
+  </si>
+  <si>
+    <t>Assemblage</t>
+  </si>
+  <si>
+    <t>Sinbuk_1</t>
   </si>
 </sst>
 </file>
@@ -1540,8 +1543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O174"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="171" workbookViewId="0">
-      <selection activeCell="D179" sqref="D179"/>
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="171" workbookViewId="0">
+      <selection activeCell="C168" sqref="C168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7" defaultRowHeight="11" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1569,7 +1572,7 @@
         <v>314</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -2641,7 +2644,7 @@
         <v>292</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>320</v>
@@ -2688,7 +2691,7 @@
         <v>292</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>321</v>
@@ -2735,7 +2738,7 @@
         <v>292</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>322</v>
@@ -2782,7 +2785,7 @@
         <v>292</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>322</v>
@@ -2829,7 +2832,7 @@
         <v>292</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>322</v>
@@ -2876,7 +2879,7 @@
         <v>292</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>322</v>
@@ -2923,7 +2926,7 @@
         <v>292</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>322</v>
@@ -2970,7 +2973,7 @@
         <v>292</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>322</v>
@@ -3017,7 +3020,7 @@
         <v>292</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>322</v>
@@ -3064,7 +3067,7 @@
         <v>292</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>322</v>
@@ -3111,7 +3114,7 @@
         <v>292</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>322</v>
@@ -3158,7 +3161,7 @@
         <v>292</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>322</v>
@@ -3205,7 +3208,7 @@
         <v>292</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>322</v>
@@ -3252,7 +3255,7 @@
         <v>292</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>322</v>
@@ -3299,7 +3302,7 @@
         <v>292</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C38" s="10" t="s">
         <v>322</v>
@@ -3346,7 +3349,7 @@
         <v>292</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C39" s="10" t="s">
         <v>323</v>
@@ -3393,7 +3396,7 @@
         <v>292</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>323</v>
@@ -3440,7 +3443,7 @@
         <v>292</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>323</v>
@@ -3487,7 +3490,7 @@
         <v>292</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C42" s="10" t="s">
         <v>323</v>
@@ -3534,7 +3537,7 @@
         <v>292</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C43" s="10" t="s">
         <v>323</v>
@@ -3581,7 +3584,7 @@
         <v>292</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>323</v>
@@ -3628,7 +3631,7 @@
         <v>292</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C45" s="10" t="s">
         <v>323</v>
@@ -3675,7 +3678,7 @@
         <v>292</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C46" s="10" t="s">
         <v>323</v>
@@ -3722,7 +3725,7 @@
         <v>292</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C47" s="10" t="s">
         <v>323</v>
@@ -3769,7 +3772,7 @@
         <v>292</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>323</v>
@@ -3816,7 +3819,7 @@
         <v>292</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>323</v>
@@ -3863,7 +3866,7 @@
         <v>292</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C50" s="10" t="s">
         <v>323</v>
@@ -3910,7 +3913,7 @@
         <v>292</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C51" s="10" t="s">
         <v>323</v>
@@ -3957,7 +3960,7 @@
         <v>292</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>323</v>
@@ -4004,7 +4007,7 @@
         <v>292</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C53" s="10" t="s">
         <v>323</v>
@@ -4051,7 +4054,7 @@
         <v>292</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C54" s="10" t="s">
         <v>323</v>
@@ -4098,7 +4101,7 @@
         <v>292</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C55" s="10" t="s">
         <v>323</v>
@@ -4145,7 +4148,7 @@
         <v>292</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C56" s="10" t="s">
         <v>323</v>
@@ -4192,7 +4195,7 @@
         <v>292</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C57" s="10" t="s">
         <v>323</v>
@@ -4239,7 +4242,7 @@
         <v>292</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C58" s="10" t="s">
         <v>323</v>
@@ -4286,7 +4289,7 @@
         <v>292</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>323</v>
@@ -4333,7 +4336,7 @@
         <v>292</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C60" s="10" t="s">
         <v>323</v>
@@ -4380,7 +4383,7 @@
         <v>292</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C61" s="10" t="s">
         <v>323</v>
@@ -4427,7 +4430,7 @@
         <v>292</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C62" s="10" t="s">
         <v>323</v>
@@ -4474,7 +4477,7 @@
         <v>292</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C63" s="10" t="s">
         <v>323</v>
@@ -4521,7 +4524,7 @@
         <v>292</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C64" s="10" t="s">
         <v>323</v>
@@ -4568,7 +4571,7 @@
         <v>292</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C65" s="10" t="s">
         <v>323</v>
@@ -4615,7 +4618,7 @@
         <v>292</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C66" s="10" t="s">
         <v>323</v>
@@ -4662,7 +4665,7 @@
         <v>292</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C67" s="10" t="s">
         <v>323</v>
@@ -4709,7 +4712,7 @@
         <v>292</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C68" s="10" t="s">
         <v>323</v>
@@ -4756,7 +4759,7 @@
         <v>292</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C69" s="10" t="s">
         <v>323</v>
@@ -4803,7 +4806,7 @@
         <v>292</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C70" s="10" t="s">
         <v>323</v>
@@ -4850,7 +4853,7 @@
         <v>292</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C71" s="10" t="s">
         <v>323</v>
@@ -4897,7 +4900,7 @@
         <v>292</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>323</v>
@@ -4944,7 +4947,7 @@
         <v>292</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C73" s="10" t="s">
         <v>323</v>
@@ -4991,7 +4994,7 @@
         <v>292</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C74" s="10" t="s">
         <v>323</v>
@@ -5038,7 +5041,7 @@
         <v>292</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C75" s="10" t="s">
         <v>323</v>
@@ -5085,7 +5088,7 @@
         <v>292</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C76" s="10" t="s">
         <v>323</v>
@@ -5132,7 +5135,7 @@
         <v>292</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C77" s="10" t="s">
         <v>323</v>
@@ -5179,7 +5182,7 @@
         <v>292</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C78" s="10" t="s">
         <v>323</v>
@@ -5226,7 +5229,7 @@
         <v>292</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C79" s="10" t="s">
         <v>323</v>
@@ -5273,7 +5276,7 @@
         <v>292</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C80" s="10" t="s">
         <v>323</v>
@@ -5320,7 +5323,7 @@
         <v>292</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C81" s="10" t="s">
         <v>323</v>
@@ -5367,7 +5370,7 @@
         <v>292</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C82" s="10" t="s">
         <v>323</v>
@@ -5414,7 +5417,7 @@
         <v>292</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C83" s="10" t="s">
         <v>323</v>
@@ -5461,7 +5464,7 @@
         <v>292</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C84" s="10" t="s">
         <v>323</v>
@@ -5508,7 +5511,7 @@
         <v>292</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C85" s="10" t="s">
         <v>323</v>
@@ -5555,7 +5558,7 @@
         <v>292</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C86" s="10" t="s">
         <v>323</v>
@@ -5602,7 +5605,7 @@
         <v>292</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C87" s="10" t="s">
         <v>323</v>
@@ -5649,7 +5652,7 @@
         <v>292</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C88" s="10" t="s">
         <v>323</v>
@@ -5696,7 +5699,7 @@
         <v>292</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C89" s="10" t="s">
         <v>323</v>
@@ -5743,7 +5746,7 @@
         <v>292</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C90" s="10" t="s">
         <v>323</v>
@@ -5790,7 +5793,7 @@
         <v>292</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C91" s="10" t="s">
         <v>323</v>
@@ -5837,7 +5840,7 @@
         <v>292</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C92" s="10" t="s">
         <v>323</v>
@@ -5884,7 +5887,7 @@
         <v>292</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C93" s="10" t="s">
         <v>323</v>
@@ -5931,7 +5934,7 @@
         <v>292</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C94" s="10" t="s">
         <v>323</v>
@@ -5978,7 +5981,7 @@
         <v>292</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C95" s="10" t="s">
         <v>323</v>
@@ -6025,7 +6028,7 @@
         <v>292</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C96" s="10" t="s">
         <v>323</v>
@@ -6072,7 +6075,7 @@
         <v>292</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C97" s="10" t="s">
         <v>323</v>
@@ -6119,7 +6122,7 @@
         <v>292</v>
       </c>
       <c r="B98" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C98" s="10" t="s">
         <v>323</v>
@@ -6166,7 +6169,7 @@
         <v>292</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C99" s="10" t="s">
         <v>323</v>
@@ -6213,7 +6216,7 @@
         <v>292</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C100" s="10" t="s">
         <v>323</v>
@@ -6260,7 +6263,7 @@
         <v>292</v>
       </c>
       <c r="B101" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C101" s="10" t="s">
         <v>323</v>
@@ -6307,7 +6310,7 @@
         <v>292</v>
       </c>
       <c r="B102" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C102" s="10" t="s">
         <v>323</v>
@@ -6354,7 +6357,7 @@
         <v>292</v>
       </c>
       <c r="B103" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C103" s="10" t="s">
         <v>323</v>
@@ -6401,7 +6404,7 @@
         <v>292</v>
       </c>
       <c r="B104" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C104" s="10" t="s">
         <v>323</v>
@@ -6448,7 +6451,7 @@
         <v>292</v>
       </c>
       <c r="B105" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C105" s="10" t="s">
         <v>323</v>
@@ -6495,7 +6498,7 @@
         <v>292</v>
       </c>
       <c r="B106" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C106" s="10" t="s">
         <v>323</v>
@@ -6542,7 +6545,7 @@
         <v>292</v>
       </c>
       <c r="B107" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C107" s="10" t="s">
         <v>323</v>
@@ -6589,7 +6592,7 @@
         <v>292</v>
       </c>
       <c r="B108" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C108" s="10" t="s">
         <v>323</v>
@@ -6636,7 +6639,7 @@
         <v>292</v>
       </c>
       <c r="B109" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C109" s="10" t="s">
         <v>323</v>
@@ -6683,7 +6686,7 @@
         <v>292</v>
       </c>
       <c r="B110" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C110" s="10" t="s">
         <v>323</v>
@@ -6730,7 +6733,7 @@
         <v>292</v>
       </c>
       <c r="B111" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C111" s="10" t="s">
         <v>323</v>
@@ -6777,7 +6780,7 @@
         <v>292</v>
       </c>
       <c r="B112" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C112" s="10" t="s">
         <v>323</v>
@@ -6824,7 +6827,7 @@
         <v>292</v>
       </c>
       <c r="B113" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C113" s="10" t="s">
         <v>323</v>
@@ -7247,7 +7250,7 @@
         <v>305</v>
       </c>
       <c r="B122" s="10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C122" s="10" t="s">
         <v>327</v>
@@ -7292,7 +7295,7 @@
         <v>305</v>
       </c>
       <c r="B123" s="10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C123" s="10" t="s">
         <v>328</v>
@@ -9393,10 +9396,10 @@
         <v>299</v>
       </c>
       <c r="B168" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C168" s="10" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>159</v>
@@ -9440,10 +9443,10 @@
         <v>299</v>
       </c>
       <c r="B169" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C169" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>162</v>
@@ -9487,10 +9490,10 @@
         <v>299</v>
       </c>
       <c r="B170" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C170" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>162</v>
@@ -9534,10 +9537,10 @@
         <v>299</v>
       </c>
       <c r="B171" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C171" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>162</v>
@@ -9581,10 +9584,10 @@
         <v>299</v>
       </c>
       <c r="B172" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C172" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>162</v>
@@ -9628,10 +9631,10 @@
         <v>299</v>
       </c>
       <c r="B173" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C173" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>162</v>
@@ -9675,10 +9678,10 @@
         <v>299</v>
       </c>
       <c r="B174" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C174" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>162</v>

</xml_diff>